<commit_message>
designs for 120mhz clk
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer8/80mhz/mxu_24x24/timing.xlsx
+++ b/dtpu_configurations/only_integer8/80mhz/mxu_24x24/timing.xlsx
@@ -119,10 +119,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>4.727475166320801</v>
+        <v>0.3036486506462097</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.01883271336555481</v>
+        <v>0.012261303141713142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>